<commit_message>
added execute flag in testprotocol
</commit_message>
<xml_diff>
--- a/test/testcases/testcase24_oracle_bigquery_counting.xlsx
+++ b/test/testcases/testcase24_oracle_bigquery_counting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\GitHub\QE_Automated_Testing_Framework\test\testcases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\GitHub\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EB4D24-3D01-413C-99C6-467F33366E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCAE381-9FC5-408F-8A20-63055D15BE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>sourcequerymode</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>indigo-almanac-384011.atf_data_source.hnpstats_data</t>
+  </si>
+  <si>
+    <t>Auto</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +579,9 @@
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">

</xml_diff>